<commit_message>
recisions on partyboat lanfings fb163
</commit_message>
<xml_diff>
--- a/data/landings/cdfw/public/fish_bulletins/raw/fb163/raw/Table22.xlsx
+++ b/data/landings/cdfw/public/fish_bulletins/raw/fb163/raw/Table22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilavargaspoulsen/github/wc_climate_synthesis/data/landings/cdfw/public/fish_bulletins/raw/fb163/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9AC1B80-0BE9-B942-B31F-EC92C81F64BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225D45F4-7D5D-4C48-AA0C-0DAB41B28753}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -114,6 +114,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -161,40 +162,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -521,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1283,16 +1284,36 @@
       <c r="A22" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
+      <c r="B22" s="3">
+        <v>695445</v>
+      </c>
+      <c r="C22" s="3">
+        <v>688103</v>
+      </c>
+      <c r="D22" s="3">
+        <v>857000</v>
+      </c>
+      <c r="E22" s="3">
+        <v>780102</v>
+      </c>
+      <c r="F22" s="3">
+        <v>849654</v>
+      </c>
+      <c r="G22" s="3">
+        <v>802811</v>
+      </c>
+      <c r="H22" s="3">
+        <v>872327</v>
+      </c>
+      <c r="I22" s="3">
+        <v>728126</v>
+      </c>
+      <c r="J22" s="3">
+        <v>792618</v>
+      </c>
+      <c r="K22" s="3">
+        <v>880100</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
anglers data 1st take
</commit_message>
<xml_diff>
--- a/data/landings/cdfw/public/fish_bulletins/raw/fb163/raw/Table22.xlsx
+++ b/data/landings/cdfw/public/fish_bulletins/raw/fb163/raw/Table22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilavargaspoulsen/github/wc_climate_synthesis/data/landings/cdfw/public/fish_bulletins/raw/fb163/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225D45F4-7D5D-4C48-AA0C-0DAB41B28753}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612E3E5C-8432-BE4C-B3DD-AA3D8A8EE364}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Total number of fish</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Salmon</t>
+  </si>
+  <si>
+    <t>w</t>
   </si>
 </sst>
 </file>
@@ -520,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1303,7 +1306,7 @@
         <v>802811</v>
       </c>
       <c r="H22" s="3">
-        <v>872327</v>
+        <v>873327</v>
       </c>
       <c r="I22" s="3">
         <v>728126</v>
@@ -1313,6 +1316,11 @@
       </c>
       <c r="K22" s="3">
         <v>880100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H23" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>